<commit_message>
Manually merging Z commit with what I've been doing at uni
</commit_message>
<xml_diff>
--- a/CW1/Results1024Home.xlsx
+++ b/CW1/Results1024Home.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Kevin1024Home" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="10">
   <si>
     <t>Image Dimensions (px)</t>
   </si>
@@ -42,11 +47,14 @@
   <si>
     <t>Average:</t>
   </si>
+  <si>
+    <t>Fixed Parallel For</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,6 +602,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -641,7 +652,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -676,7 +687,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -887,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="O148" sqref="O148:P148"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="N147" sqref="N147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,7 +3545,7 @@
         <v>5</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O113" s="1" t="s">
         <v>7</v>
@@ -3695,6 +3706,20 @@
         <v>881369</v>
       </c>
       <c r="Q120" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N121" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O121" s="2">
+        <v>256</v>
+      </c>
+      <c r="P121" s="2">
+        <v>850717</v>
+      </c>
+      <c r="Q121" s="2">
         <v>9</v>
       </c>
     </row>
@@ -3718,10 +3743,24 @@
       </c>
       <c r="P124" s="2">
         <f>AVERAGE(P114:P123)</f>
-        <v>878189.85714285716</v>
-      </c>
-    </row>
-    <row r="136" spans="3:16" x14ac:dyDescent="0.25">
+        <v>874755.75</v>
+      </c>
+    </row>
+    <row r="135" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="N135" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O135" s="2">
+        <v>256</v>
+      </c>
+      <c r="P135" s="2">
+        <v>805825</v>
+      </c>
+      <c r="Q135" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C136" s="3" t="s">
         <v>8</v>
       </c>
@@ -3739,9 +3778,9 @@
       <c r="O136" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P136" s="2" t="e">
+      <c r="P136" s="2">
         <f>AVERAGE(P126:P135)</f>
-        <v>#DIV/0!</v>
+        <v>805825</v>
       </c>
     </row>
     <row r="148" spans="3:16" x14ac:dyDescent="0.25">

</xml_diff>